<commit_message>
synced to new excel form
</commit_message>
<xml_diff>
--- a/src/Resource/levelData.xlsx
+++ b/src/Resource/levelData.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="28035" windowHeight="13680"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="24960" windowHeight="15060"/>
   </bookViews>
   <sheets>
     <sheet name="怪物表" sheetId="1" r:id="rId1"/>
     <sheet name="奖励组" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>怪物ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -110,14 +115,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>刀兵</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>飞刀兵</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>刀盾兵</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -138,23 +135,47 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>{"speed":300,"dir":[0,1]}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>{"speed":250}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>{"speed":200,"loops":[[1,2],[2,3],[4,5]]}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"speed":200,"dir":[0,1]}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"gap":3.5,"id":15000}</t>
+    <t>弓箭手</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"speed":300,"dir":[0,-1]}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"speed":300,"dir":[0,-1]}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOSS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>子弹</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"speed":300}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>子弹2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"gap":4,"id":50000}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"gap":2.5,"id":50001}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"speed":150,"loops":[[100, 700], [320, 600], [540, 700]]}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -162,7 +183,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +224,24 @@
       <sz val="9"/>
       <name val="宋体"/>
       <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -346,8 +385,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -429,8 +498,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="11">
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -729,23 +808,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="10" max="10" width="22.375" customWidth="1"/>
-    <col min="11" max="11" width="23.25" customWidth="1"/>
-    <col min="16" max="16" width="14.375" customWidth="1"/>
-    <col min="17" max="17" width="13.875" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" customWidth="1"/>
+    <col min="11" max="11" width="23.1640625" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" customWidth="1"/>
+    <col min="17" max="17" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="12" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="12" customFormat="1" ht="15">
       <c r="A1" s="22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -766,11 +845,11 @@
       <c r="N1" s="23"/>
       <c r="O1" s="23"/>
       <c r="P1" s="20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Q1" s="21"/>
     </row>
-    <row r="2" spans="1:17" s="13" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" s="13" customFormat="1" ht="16">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -815,7 +894,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="13" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" s="13" customFormat="1" ht="16">
       <c r="A3" s="4">
         <v>11000</v>
       </c>
@@ -858,12 +937,12 @@
         <v>8001</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="13" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" s="13" customFormat="1" ht="16">
       <c r="A4" s="4">
-        <v>12000</v>
+        <v>40000</v>
       </c>
       <c r="B4" s="4">
-        <v>1003</v>
+        <v>4001</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>22</v>
@@ -899,12 +978,12 @@
         <v>8002</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="13" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" s="13" customFormat="1" ht="16">
       <c r="A5" s="4">
         <v>13000</v>
       </c>
       <c r="B5" s="4">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>23</v>
@@ -916,7 +995,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G5" s="16"/>
       <c r="H5" s="16"/>
@@ -942,34 +1021,34 @@
         <v>8003</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="13" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" s="13" customFormat="1" ht="16">
       <c r="A6" s="4">
         <v>14000</v>
       </c>
       <c r="B6" s="4">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D6" s="18">
         <v>1</v>
       </c>
       <c r="E6" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
       <c r="J6" s="17"/>
       <c r="K6" s="19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L6" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M6" s="4">
         <v>10</v>
@@ -987,50 +1066,137 @@
         <v>8004</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="13" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" s="13" customFormat="1" ht="16">
       <c r="A7" s="4">
-        <v>15000</v>
+        <v>20000</v>
       </c>
       <c r="B7" s="4">
-        <v>1002</v>
+        <v>2001</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D7" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
       <c r="J7" s="17"/>
-      <c r="K7" s="18"/>
+      <c r="K7" s="19" t="s">
+        <v>37</v>
+      </c>
       <c r="L7" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M7" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="N7" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O7" s="4">
         <v>0</v>
       </c>
       <c r="P7" s="6">
-        <v>7005</v>
+        <v>7004</v>
       </c>
       <c r="Q7" s="6">
-        <v>8005</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" s="13" customFormat="1" ht="16.5" x14ac:dyDescent="0.15"/>
+        <v>8004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" s="13" customFormat="1" ht="16">
+      <c r="A8" s="4">
+        <v>50000</v>
+      </c>
+      <c r="B8" s="4">
+        <v>5001</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="18">
+        <v>0</v>
+      </c>
+      <c r="E8" s="18">
+        <v>4</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="4">
+        <v>1</v>
+      </c>
+      <c r="M8" s="4">
+        <v>1</v>
+      </c>
+      <c r="N8" s="4">
+        <v>1</v>
+      </c>
+      <c r="O8" s="4">
+        <v>0</v>
+      </c>
+      <c r="P8" s="6">
+        <v>7004</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>8004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" s="13" customFormat="1" ht="16">
+      <c r="A9" s="4">
+        <v>50001</v>
+      </c>
+      <c r="B9" s="4">
+        <v>5002</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="18">
+        <v>0</v>
+      </c>
+      <c r="E9" s="18">
+        <v>4</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="4">
+        <v>1</v>
+      </c>
+      <c r="M9" s="4">
+        <v>1</v>
+      </c>
+      <c r="N9" s="4">
+        <v>2</v>
+      </c>
+      <c r="O9" s="4">
+        <v>0</v>
+      </c>
+      <c r="P9" s="6">
+        <v>7004</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>8004</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="P1:Q1"/>
@@ -1040,7 +1206,12 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1052,9 +1223,9 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1064,7 +1235,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
@@ -1078,13 +1249,13 @@
         <v>15</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="12" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="12" customFormat="1" ht="15">
       <c r="A3" s="6">
         <v>7001</v>
       </c>
@@ -1100,7 +1271,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" s="12" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" s="12" customFormat="1" ht="15">
       <c r="A4" s="6">
         <v>7002</v>
       </c>
@@ -1116,7 +1287,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" s="12" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" s="12" customFormat="1" ht="15">
       <c r="A5" s="6">
         <v>7003</v>
       </c>
@@ -1132,7 +1303,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" s="12" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" s="12" customFormat="1" ht="15">
       <c r="A6" s="6">
         <v>7004</v>
       </c>
@@ -1148,7 +1319,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" s="12" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" s="12" customFormat="1" ht="15">
       <c r="A7" s="6">
         <v>7005</v>
       </c>
@@ -1164,7 +1335,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15">
       <c r="A8" s="25">
         <v>8001</v>
       </c>
@@ -1182,7 +1353,7 @@
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15">
       <c r="A9" s="26"/>
       <c r="B9" s="4">
         <v>50</v>
@@ -1194,7 +1365,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15">
       <c r="A10" s="25">
         <v>8002</v>
       </c>
@@ -1212,7 +1383,7 @@
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15">
       <c r="A11" s="27"/>
       <c r="B11" s="4">
         <v>20</v>
@@ -1228,7 +1399,7 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="15">
       <c r="A12" s="27"/>
       <c r="B12" s="4">
         <v>10</v>
@@ -1244,7 +1415,7 @@
       </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15">
       <c r="A13" s="27"/>
       <c r="B13" s="4">
         <v>10</v>
@@ -1260,7 +1431,7 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15">
       <c r="A14" s="26"/>
       <c r="B14" s="4">
         <v>10</v>
@@ -1276,7 +1447,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="15">
       <c r="A15" s="25">
         <v>8003</v>
       </c>
@@ -1294,7 +1465,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="15">
       <c r="A16" s="27"/>
       <c r="B16" s="4">
         <v>30</v>
@@ -1310,7 +1481,7 @@
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="15">
       <c r="A17" s="26"/>
       <c r="B17" s="4">
         <v>30</v>
@@ -1326,7 +1497,7 @@
       </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="15">
       <c r="A18" s="4">
         <v>8004</v>
       </c>
@@ -1344,7 +1515,7 @@
       </c>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="15">
       <c r="A19" s="25">
         <v>8005</v>
       </c>
@@ -1362,7 +1533,7 @@
       </c>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="15">
       <c r="A20" s="27"/>
       <c r="B20" s="4">
         <v>30</v>
@@ -1378,7 +1549,7 @@
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="15">
       <c r="A21" s="26"/>
       <c r="B21" s="4">
         <v>30</v>
@@ -1403,7 +1574,12 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1415,9 +1591,14 @@
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix some user exp
</commit_message>
<xml_diff>
--- a/src/Resource/levelData.xlsx
+++ b/src/Resource/levelData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="36920" windowHeight="23560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29040" windowHeight="18240"/>
   </bookViews>
   <sheets>
     <sheet name="怪物表" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
   <si>
     <t>怪物ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -135,47 +135,80 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>弓箭手</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOSS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>子弹</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>子弹2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>qiangbing</t>
+  </si>
+  <si>
+    <t>daodunbing</t>
+  </si>
+  <si>
+    <t>gongjianshou</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>{"speed":300,"dir":[0,-1]}</t>
+  </si>
+  <si>
+    <t>{"interval":1,"radius":100}</t>
+  </si>
+  <si>
     <t>{"speed":250}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>弓箭手</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"speed":300,"dir":[0,-1]}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"speed":300,"dir":[0,-1]}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BOSS</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>子弹</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>{"interval":2.5,"bullet":50000,"radius":1000}</t>
+  </si>
+  <si>
+    <t>{"speed":150,"loop":[[100, 700], [320, 600], [540, 700]]}</t>
+  </si>
+  <si>
+    <t>{"interval":2.5,"bullet":50001,"radius":1000}</t>
   </si>
   <si>
     <t>{"speed":300}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>子弹2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"gap":4,"id":50000}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"gap":2.5,"id":50001}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"speed":150,"loop":[[100, 700], [320, 600], [540, 700]]}</t>
+  </si>
+  <si>
+    <t>{"radius":1}</t>
+  </si>
+  <si>
+    <t>StayOnMap</t>
+  </si>
+  <si>
+    <t>MoveDirectionAndAttack</t>
+  </si>
+  <si>
+    <t>ChaseAndAttack</t>
+  </si>
+  <si>
+    <t>MoveLoopAndAttack</t>
+  </si>
+  <si>
+    <t>CustomPathStopAtExit</t>
+  </si>
+  <si>
+    <t>CustomPathTangentExit</t>
+  </si>
+  <si>
+    <t>{"speed":300}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -183,7 +216,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +278,12 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -420,7 +459,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -497,19 +536,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -808,21 +850,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="10" max="10" width="22.33203125" customWidth="1"/>
-    <col min="11" max="11" width="23.1640625" customWidth="1"/>
-    <col min="16" max="16" width="14.33203125" customWidth="1"/>
-    <col min="17" max="17" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="10" max="10" width="22.375" customWidth="1"/>
+    <col min="11" max="11" width="23.125" customWidth="1"/>
+    <col min="16" max="16" width="14.375" customWidth="1"/>
+    <col min="17" max="17" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="12" customFormat="1" ht="15">
+    <row r="1" spans="1:17" s="12" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
         <v>24</v>
       </c>
@@ -849,7 +892,7 @@
       </c>
       <c r="Q1" s="21"/>
     </row>
-    <row r="2" spans="1:17" s="13" customFormat="1" ht="16">
+    <row r="2" spans="1:17" s="13" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -894,30 +937,32 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="13" customFormat="1" ht="16">
+    <row r="3" spans="1:17" s="13" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>11000</v>
       </c>
-      <c r="B3" s="4">
-        <v>1001</v>
+      <c r="B3" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="14">
-        <v>0</v>
-      </c>
-      <c r="E3" s="14">
-        <v>1</v>
+      <c r="D3" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>46</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
       <c r="J3" s="17"/>
-      <c r="K3" s="18"/>
+      <c r="K3" s="18" t="s">
+        <v>37</v>
+      </c>
       <c r="L3" s="4">
         <v>1</v>
       </c>
@@ -937,7 +982,7 @@
         <v>8001</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="13" customFormat="1" ht="16">
+    <row r="4" spans="1:17" s="13" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>40000</v>
       </c>
@@ -947,11 +992,9 @@
       <c r="C4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="18">
-        <v>0</v>
-      </c>
-      <c r="E4" s="18">
-        <v>0</v>
+      <c r="D4" s="18"/>
+      <c r="E4" s="28" t="s">
+        <v>45</v>
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="16"/>
@@ -978,30 +1021,32 @@
         <v>8002</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="13" customFormat="1" ht="16">
+    <row r="5" spans="1:17" s="13" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>13000</v>
       </c>
-      <c r="B5" s="4">
-        <v>1002</v>
+      <c r="B5" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="18">
-        <v>0</v>
-      </c>
-      <c r="E5" s="18">
-        <v>3</v>
+      <c r="D5" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>47</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="G5" s="16"/>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
       <c r="J5" s="17"/>
-      <c r="K5" s="18"/>
+      <c r="K5" s="18" t="s">
+        <v>37</v>
+      </c>
       <c r="L5" s="4">
         <v>2</v>
       </c>
@@ -1021,31 +1066,31 @@
         <v>8003</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="13" customFormat="1" ht="16">
+    <row r="6" spans="1:17" s="13" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>14000</v>
       </c>
-      <c r="B6" s="4">
-        <v>1003</v>
+      <c r="B6" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="18">
-        <v>1</v>
-      </c>
-      <c r="E6" s="18">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>46</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
       <c r="J6" s="17"/>
       <c r="K6" s="19" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="L6" s="4">
         <v>3</v>
@@ -1066,7 +1111,7 @@
         <v>8004</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="13" customFormat="1" ht="16">
+    <row r="7" spans="1:17" s="13" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>20000</v>
       </c>
@@ -1074,23 +1119,23 @@
         <v>2001</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="18">
-        <v>1</v>
-      </c>
-      <c r="E7" s="18">
-        <v>2</v>
+        <v>29</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>48</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
       <c r="J7" s="17"/>
       <c r="K7" s="19" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="L7" s="4">
         <v>3</v>
@@ -1111,7 +1156,7 @@
         <v>8004</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="13" customFormat="1" ht="16">
+    <row r="8" spans="1:17" s="13" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>50000</v>
       </c>
@@ -1119,22 +1164,24 @@
         <v>5001</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="18">
-        <v>0</v>
-      </c>
-      <c r="E8" s="18">
-        <v>4</v>
+        <v>30</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>47</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
       <c r="I8" s="16"/>
       <c r="J8" s="17"/>
-      <c r="K8" s="19"/>
+      <c r="K8" s="19" t="s">
+        <v>44</v>
+      </c>
       <c r="L8" s="4">
         <v>1</v>
       </c>
@@ -1154,7 +1201,7 @@
         <v>8004</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="13" customFormat="1" ht="16">
+    <row r="9" spans="1:17" s="13" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>50001</v>
       </c>
@@ -1162,22 +1209,24 @@
         <v>5002</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="18">
-        <v>0</v>
-      </c>
-      <c r="E9" s="18">
-        <v>4</v>
+      <c r="E9" s="28" t="s">
+        <v>47</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
       <c r="J9" s="17"/>
-      <c r="K9" s="19"/>
+      <c r="K9" s="19" t="s">
+        <v>44</v>
+      </c>
       <c r="L9" s="4">
         <v>1</v>
       </c>
@@ -1195,6 +1244,96 @@
       </c>
       <c r="Q9" s="6">
         <v>8004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" s="13" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
+        <v>15000</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="4">
+        <v>3</v>
+      </c>
+      <c r="M10" s="4">
+        <v>10</v>
+      </c>
+      <c r="N10" s="4">
+        <v>3</v>
+      </c>
+      <c r="O10" s="4">
+        <v>0</v>
+      </c>
+      <c r="P10" s="6">
+        <v>7004</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>8004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" s="13" customFormat="1" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
+        <v>16000</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="L11" s="4">
+        <v>2</v>
+      </c>
+      <c r="M11" s="4">
+        <v>3</v>
+      </c>
+      <c r="N11" s="4">
+        <v>2</v>
+      </c>
+      <c r="O11" s="4">
+        <v>0</v>
+      </c>
+      <c r="P11" s="6">
+        <v>7003</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>8003</v>
       </c>
     </row>
   </sheetData>
@@ -1206,7 +1345,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1223,9 +1362,9 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15">
+    <row r="1" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1235,7 +1374,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="15">
+    <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
@@ -1255,7 +1394,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="12" customFormat="1" ht="15">
+    <row r="3" spans="1:6" s="12" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A3" s="6">
         <v>7001</v>
       </c>
@@ -1271,7 +1410,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" s="12" customFormat="1" ht="15">
+    <row r="4" spans="1:6" s="12" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A4" s="6">
         <v>7002</v>
       </c>
@@ -1287,7 +1426,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" s="12" customFormat="1" ht="15">
+    <row r="5" spans="1:6" s="12" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A5" s="6">
         <v>7003</v>
       </c>
@@ -1303,7 +1442,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" s="12" customFormat="1" ht="15">
+    <row r="6" spans="1:6" s="12" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A6" s="6">
         <v>7004</v>
       </c>
@@ -1319,7 +1458,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" s="12" customFormat="1" ht="15">
+    <row r="7" spans="1:6" s="12" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A7" s="6">
         <v>7005</v>
       </c>
@@ -1335,7 +1474,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="15">
+    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A8" s="25">
         <v>8001</v>
       </c>
@@ -1353,7 +1492,7 @@
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="15">
+    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A9" s="26"/>
       <c r="B9" s="4">
         <v>50</v>
@@ -1365,7 +1504,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="15">
+    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A10" s="25">
         <v>8002</v>
       </c>
@@ -1383,7 +1522,7 @@
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="15">
+    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A11" s="27"/>
       <c r="B11" s="4">
         <v>20</v>
@@ -1399,7 +1538,7 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="15">
+    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A12" s="27"/>
       <c r="B12" s="4">
         <v>10</v>
@@ -1415,7 +1554,7 @@
       </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="15">
+    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A13" s="27"/>
       <c r="B13" s="4">
         <v>10</v>
@@ -1431,7 +1570,7 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="15">
+    <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A14" s="26"/>
       <c r="B14" s="4">
         <v>10</v>
@@ -1447,7 +1586,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="15">
+    <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A15" s="25">
         <v>8003</v>
       </c>
@@ -1465,7 +1604,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="15">
+    <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A16" s="27"/>
       <c r="B16" s="4">
         <v>30</v>
@@ -1481,7 +1620,7 @@
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="15">
+    <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A17" s="26"/>
       <c r="B17" s="4">
         <v>30</v>
@@ -1497,7 +1636,7 @@
       </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="15">
+    <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>8004</v>
       </c>
@@ -1515,7 +1654,7 @@
       </c>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="15">
+    <row r="19" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A19" s="25">
         <v>8005</v>
       </c>
@@ -1533,7 +1672,7 @@
       </c>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="15">
+    <row r="20" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A20" s="27"/>
       <c r="B20" s="4">
         <v>30</v>
@@ -1549,7 +1688,7 @@
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="15">
+    <row r="21" spans="1:6" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A21" s="26"/>
       <c r="B21" s="4">
         <v>30</v>
@@ -1591,7 +1730,7 @@
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>